<commit_message>
finished question 9, returning to 7b
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emily\Documents\NSS_Analytics_Bootcamp\Excel\lookups-exercise-eemchadwick\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{334B2538-5967-41AE-A93D-2368B302766E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA95FE4D-EDB5-49A6-82A1-799E8DCD3265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28395" yWindow="-840" windowWidth="26235" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2195,8 +2195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="D98" sqref="D98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5871,27 +5871,90 @@
       <c r="A98" t="s">
         <v>73</v>
       </c>
-      <c r="C98" s="4"/>
-      <c r="E98" s="4"/>
-      <c r="G98" s="4"/>
+      <c r="B98" t="str">
+        <f>INDEX($A$2:$A$52, MATCH($B$96, F$2:F$52,0))</f>
+        <v>Clerk and Master - Chancery</v>
+      </c>
+      <c r="C98" s="5">
+        <f>INDEX($E$2:$E$52, MATCH($B$96, F$2:F$52,0))</f>
+        <v>-0.15235918433091292</v>
+      </c>
+      <c r="D98" t="str">
+        <f>INDEX($A$2:$A$52, MATCH($D$96, F$2:F$52,0))</f>
+        <v>Circuit Court Clerk</v>
+      </c>
+      <c r="E98" s="5">
+        <f>INDEX($E$2:$E$52, MATCH(D$96, F$2:F$52,0))</f>
+        <v>-0.11502817362571344</v>
+      </c>
+      <c r="F98" t="str">
+        <f>INDEX($A$2:$A$52, MATCH($F$96, F$2:F$52,0))</f>
+        <v>Internal Audit</v>
+      </c>
+      <c r="G98" s="5">
+        <f>INDEX($E$2:$E$52, MATCH(F$96, F$2:F$52,0))</f>
+        <v>-9.5782760864849215E-2</v>
+      </c>
       <c r="I98" s="4"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>74</v>
       </c>
-      <c r="C99" s="4"/>
-      <c r="E99" s="4"/>
-      <c r="G99" s="4"/>
+      <c r="B99" t="str">
+        <f>INDEX($A$2:$A$52, MATCH($B$96, K$2:K$52,0))</f>
+        <v>Metropolitan Clerk</v>
+      </c>
+      <c r="C99" s="5">
+        <f>INDEX($J$2:$J$52, MATCH($B$96, K$2:K$52,0))</f>
+        <v>-0.17551246244575608</v>
+      </c>
+      <c r="D99" t="str">
+        <f>INDEX($A$2:$A$52, MATCH($D$96, K$2:K$52,0))</f>
+        <v>Internal Audit</v>
+      </c>
+      <c r="E99" s="5">
+        <f>INDEX($J$2:$J$52, MATCH($D$96, K$2:K$52,0))</f>
+        <v>-0.17103239309050916</v>
+      </c>
+      <c r="F99" t="str">
+        <f>INDEX($A$2:$A$52, MATCH($F$96, K$2:K$52,0))</f>
+        <v>Office of Family Safety</v>
+      </c>
+      <c r="G99" s="5">
+        <f>INDEX($J$2:$J$52, MATCH($F$96, K$2:K$52,0))</f>
+        <v>-0.13918241656366656</v>
+      </c>
       <c r="I99" s="4"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>75</v>
       </c>
-      <c r="C100" s="4"/>
-      <c r="E100" s="4"/>
-      <c r="G100" s="4"/>
+      <c r="B100" t="str">
+        <f>INDEX($A$2:$A$52, MATCH($B$96, P$2:P$52,0))</f>
+        <v>Community Oversight Board</v>
+      </c>
+      <c r="C100" s="5">
+        <f>INDEX($O$2:$O$52, MATCH($B$96, P$2:P$52,0))</f>
+        <v>-0.82994157333333329</v>
+      </c>
+      <c r="D100" t="str">
+        <f>INDEX($A$2:$A$52, MATCH($D$96, P$2:P$52,0))</f>
+        <v>Clerk and Master - Chancery</v>
+      </c>
+      <c r="E100" s="5">
+        <f>INDEX($O$2:$O$52, MATCH($D$96, P$2:P$52,0))</f>
+        <v>-0.15295680364719175</v>
+      </c>
+      <c r="F100" t="str">
+        <f>INDEX($A$2:$A$52, MATCH($F$96, P$2:P$52,0))</f>
+        <v>Election Commission</v>
+      </c>
+      <c r="G100" s="5">
+        <f>INDEX($O$2:$O$52, MATCH($F$96, P$2:P$52,0))</f>
+        <v>-0.12882667147667154</v>
+      </c>
       <c r="I100" s="4"/>
     </row>
   </sheetData>

</xml_diff>